<commit_message>
adding jessen and simon
</commit_message>
<xml_diff>
--- a/BETA/TA_DB_info/science_quiz_TAs.xlsx
+++ b/BETA/TA_DB_info/science_quiz_TAs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rk2643/pfb2023_fork/pfb2024/bestie files/TA_DB_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rk2643/pfb2023_fork/pfb2024/bestie files/Bestie-Bubble/BETA/TA_DB_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC25C6F-0125-4247-9AEC-476B071B030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57473F11-32B4-5A4C-86EF-92347AD122F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{A0112F70-1761-BA42-AA1E-A566A71B7164}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Robert</t>
+  </si>
+  <si>
+    <t>Jessen</t>
+  </si>
+  <si>
+    <t>Simon</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,13 +200,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACADED3-3C82-2F48-93B3-BD8DF8FB6E8A}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +688,73 @@
         <v>34</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8" xr:uid="{80FCB74B-623E-A447-A1BA-F42139A401FB}">
+      <formula1>"Sequencing,Microscopy,Flow Cytometry,Western Blot,Coding"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8" xr:uid="{12100669-0E73-6B4A-8A5C-A2A07C33CBC7}">
+      <formula1>"Human,Mouse,Arabidopsis,Fly,Worm,Yeast,Zebrafish,Non-Model Organism"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{B50FAA22-7486-E645-BE04-50DAE109E684}">
+      <formula1>"Lots,Some,Minimal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{8B460975-0D0B-874E-921F-0656679500DA}">
+      <formula1>"Wet,Dry,Both"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{F1221EC4-73E6-4E4A-8854-9FEBF2227921}">
+      <formula1>"Molecular Biology,Chemistry,Neuroscience,Ecology,Bioinformatics"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{26B09EBF-ED3A-124C-842F-6CFC7A92DBC0}">
+      <formula1>"North East,South,Midwest,West"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
@@ -676,37 +764,37 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B4 B7:B28</xm:sqref>
+          <xm:sqref>B2:B4 B9:B28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{82D39625-5F08-504E-9B7A-402A6F6875F8}">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C4 C7:C33</xm:sqref>
+          <xm:sqref>C2:C4 C9:C33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{42319ACB-E9FA-C74B-A4FA-2DC0D78C81DC}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D4 D7:D39</xm:sqref>
+          <xm:sqref>D2:D4 D9:D39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{8F04BF59-D3E7-9240-8484-55719F92847E}">
           <x14:formula1>
             <xm:f>Sheet2!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E4 E7:E86</xm:sqref>
+          <xm:sqref>E2:E4 E9:E86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCD93BE4-D742-0842-8F9C-995EBDD471B8}">
           <x14:formula1>
             <xm:f>Sheet2!$E$2:$E$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F4 F7:F63</xm:sqref>
+          <xm:sqref>F2:F4 F9:F63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D1E443CF-20FB-B045-A0B6-6CFD78CA4CFC}">
           <x14:formula1>
             <xm:f>Sheet2!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G4 G7:G144</xm:sqref>
+          <xm:sqref>G2:G4 G9:G144</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>